<commit_message>
List of Components for this project and cost
update in file disclaimer
</commit_message>
<xml_diff>
--- a/Project Components and Expenditure.xlsx
+++ b/Project Components and Expenditure.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>PiCycle SEAT Expenditure Sheet</t>
   </si>
@@ -143,7 +143,10 @@
     <t>Please note that this includes buying a Raspberry Pi. This was purchased as the 1st generation of the Rpi supplied for the project was not adequate.</t>
   </si>
   <si>
-    <t>Links have been provided where we purchased these items. No guarantee that the prices will be the same after the date of completion for this project. We cannot take any responsibilty for purchases that you make from these URLs provided</t>
+    <t xml:space="preserve">Links have been provided where we purchased these items. No guarantee that the prices will be the same after the date of completion for this project. </t>
+  </si>
+  <si>
+    <t>We cannot take any responsibilty for purchases that you make from these URLs provided</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -596,6 +599,11 @@
         <v>39</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>1</v>

</xml_diff>